<commit_message>
cambio en python de errores en las pruebas con duplicados y primary keys
</commit_message>
<xml_diff>
--- a/Excels/Organigrama Proyectos Informacional BBVA.xlsx
+++ b/Excels/Organigrama Proyectos Informacional BBVA.xlsx
@@ -5,7 +5,7 @@
   <workbookPr hidePivotFieldList="1" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmartino\Desktop\PRUEBAS BM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lmartino\Desktop\BlackMargin\MarginBlack\Excels\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,9 +29,9 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId7"/>
-    <pivotCache cacheId="1" r:id="rId8"/>
-    <pivotCache cacheId="2" r:id="rId9"/>
+    <pivotCache cacheId="3" r:id="rId7"/>
+    <pivotCache cacheId="4" r:id="rId8"/>
+    <pivotCache cacheId="5" r:id="rId9"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -3933,7 +3933,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3969,7 +3969,7 @@
         <xdr:cNvPr id="5" name="4 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0400-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0400-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4010,7 +4010,7 @@
         <xdr:cNvPr id="2" name="1 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4046,7 +4046,7 @@
         <xdr:cNvPr id="4" name="3 Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -13700,7 +13700,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica2" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="5">
   <location ref="A4:B7" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
@@ -13795,7 +13795,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica3" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="7">
   <location ref="A29:B33" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
@@ -13902,7 +13902,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica1" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="B7:C10" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="20">
     <pivotField showAll="0"/>
@@ -14005,7 +14005,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica5" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Tabla dinámica5" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="5" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="B23:C30" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" showAll="0" sortType="ascending">
@@ -14402,7 +14402,7 @@
     <col min="17" max="16384" width="9.1796875" style="61"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" s="68" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" s="68" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A1" s="66" t="s">
         <v>279</v>
       </c>
@@ -14455,7 +14455,7 @@
         <v>747</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A2" s="80">
         <v>1265</v>
       </c>
@@ -14504,7 +14504,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A3" s="80">
         <v>3809</v>
       </c>
@@ -14556,7 +14556,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A4" s="80">
         <v>3955</v>
       </c>
@@ -14608,7 +14608,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A5" s="80">
         <v>5784</v>
       </c>
@@ -14635,7 +14635,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A6" s="80">
         <v>6951</v>
       </c>
@@ -14684,7 +14684,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A7" s="80">
         <v>7170</v>
       </c>
@@ -14715,7 +14715,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A8" s="80">
         <v>7374</v>
       </c>
@@ -14742,7 +14742,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="14.25" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A9" s="80">
         <v>33503</v>
       </c>
@@ -14791,7 +14791,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A10" s="80">
         <v>33537</v>
       </c>
@@ -14843,7 +14843,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="11" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A11" s="69">
         <v>156213</v>
       </c>
@@ -14894,7 +14894,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="12" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A12" s="69">
         <v>157371</v>
       </c>
@@ -14945,7 +14945,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A13" s="80">
         <v>33901</v>
       </c>
@@ -14997,7 +14997,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="14" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A14" s="80">
         <v>101547</v>
       </c>
@@ -15049,7 +15049,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="15" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A15" s="80">
         <v>101777</v>
       </c>
@@ -15101,7 +15101,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="16" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A16" s="80">
         <v>101963</v>
       </c>
@@ -15144,7 +15144,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="17" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A17" s="80">
         <v>102159</v>
       </c>
@@ -15196,7 +15196,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="18" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A18" s="80">
         <v>103822</v>
       </c>
@@ -15248,7 +15248,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="19" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A19" s="80">
         <v>103989</v>
       </c>
@@ -15279,7 +15279,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="20" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A20" s="80">
         <v>106601</v>
       </c>
@@ -15331,7 +15331,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A21" s="80">
         <v>106810</v>
       </c>
@@ -15383,7 +15383,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="22" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A22" s="80">
         <v>107484</v>
       </c>
@@ -15412,7 +15412,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="23" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A23" s="80">
         <v>107672</v>
       </c>
@@ -15464,7 +15464,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="24" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A24" s="80">
         <v>107948</v>
       </c>
@@ -15511,7 +15511,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="25" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A25" s="80">
         <v>108049</v>
       </c>
@@ -15563,7 +15563,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="26" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A26" s="80">
         <v>108229</v>
       </c>
@@ -15615,7 +15615,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="27" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A27" s="80">
         <v>108465</v>
       </c>
@@ -15667,7 +15667,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="28" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A28" s="80">
         <v>113713</v>
       </c>
@@ -15719,7 +15719,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="29" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A29" s="80">
         <v>118336</v>
       </c>
@@ -15771,7 +15771,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="30" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A30" s="80">
         <v>121943</v>
       </c>
@@ -15823,7 +15823,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="31" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A31" s="80">
         <v>122611</v>
       </c>
@@ -15875,7 +15875,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="32" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A32" s="69"/>
       <c r="B32" s="75" t="s">
         <v>288</v>
@@ -15911,7 +15911,7 @@
       <c r="O32" s="77"/>
       <c r="P32" s="77"/>
     </row>
-    <row r="33" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A33" s="69"/>
       <c r="B33" s="75" t="s">
         <v>295</v>
@@ -15947,7 +15947,7 @@
       <c r="O33" s="77"/>
       <c r="P33" s="77"/>
     </row>
-    <row r="34" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A34" s="69"/>
       <c r="B34" s="75" t="s">
         <v>295</v>
@@ -15983,7 +15983,7 @@
       <c r="O34" s="77"/>
       <c r="P34" s="77"/>
     </row>
-    <row r="35" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A35" s="69"/>
       <c r="B35" s="75" t="s">
         <v>295</v>
@@ -16019,7 +16019,7 @@
       <c r="O35" s="77"/>
       <c r="P35" s="77"/>
     </row>
-    <row r="36" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A36" s="69"/>
       <c r="B36" s="75" t="s">
         <v>295</v>
@@ -16063,7 +16063,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A37" s="69"/>
       <c r="B37" s="75" t="s">
         <v>302</v>
@@ -16099,7 +16099,7 @@
       <c r="O37" s="77"/>
       <c r="P37" s="77"/>
     </row>
-    <row r="38" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A38" s="69"/>
       <c r="B38" s="75" t="s">
         <v>310</v>
@@ -16135,7 +16135,7 @@
       <c r="O38" s="77"/>
       <c r="P38" s="77"/>
     </row>
-    <row r="39" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A39" s="69"/>
       <c r="B39" s="75" t="s">
         <v>308</v>
@@ -16171,7 +16171,7 @@
       <c r="O39" s="77"/>
       <c r="P39" s="77"/>
     </row>
-    <row r="40" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A40" s="69"/>
       <c r="B40" s="75" t="s">
         <v>308</v>
@@ -16207,7 +16207,7 @@
       <c r="O40" s="77"/>
       <c r="P40" s="77"/>
     </row>
-    <row r="41" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A41" s="69"/>
       <c r="B41" s="75" t="s">
         <v>589</v>
@@ -16243,7 +16243,7 @@
       <c r="O41" s="77"/>
       <c r="P41" s="77"/>
     </row>
-    <row r="42" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A42" s="69"/>
       <c r="B42" s="75" t="s">
         <v>664</v>
@@ -16279,7 +16279,7 @@
       <c r="O42" s="77"/>
       <c r="P42" s="77"/>
     </row>
-    <row r="43" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A43" s="69"/>
       <c r="B43" s="75" t="s">
         <v>664</v>
@@ -16315,7 +16315,7 @@
       <c r="O43" s="77"/>
       <c r="P43" s="77"/>
     </row>
-    <row r="44" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A44" s="69"/>
       <c r="B44" s="75" t="s">
         <v>322</v>
@@ -16351,7 +16351,7 @@
       <c r="O44" s="77"/>
       <c r="P44" s="77"/>
     </row>
-    <row r="45" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A45" s="69"/>
       <c r="B45" s="75" t="s">
         <v>322</v>
@@ -16387,7 +16387,7 @@
       <c r="O45" s="77"/>
       <c r="P45" s="77"/>
     </row>
-    <row r="46" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A46" s="69"/>
       <c r="B46" s="75" t="s">
         <v>328</v>
@@ -16423,7 +16423,7 @@
       <c r="O46" s="77"/>
       <c r="P46" s="77"/>
     </row>
-    <row r="47" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A47" s="69"/>
       <c r="B47" s="75" t="s">
         <v>332</v>
@@ -16459,7 +16459,7 @@
       <c r="O47" s="77"/>
       <c r="P47" s="77"/>
     </row>
-    <row r="48" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A48" s="69"/>
       <c r="B48" s="75" t="s">
         <v>334</v>
@@ -16495,7 +16495,7 @@
       <c r="O48" s="77"/>
       <c r="P48" s="77"/>
     </row>
-    <row r="49" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A49" s="69"/>
       <c r="B49" s="75" t="s">
         <v>340</v>
@@ -16531,7 +16531,7 @@
       <c r="O49" s="77"/>
       <c r="P49" s="77"/>
     </row>
-    <row r="50" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A50" s="69"/>
       <c r="B50" s="75" t="s">
         <v>340</v>
@@ -16567,7 +16567,7 @@
       <c r="O50" s="77"/>
       <c r="P50" s="77"/>
     </row>
-    <row r="51" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A51" s="69"/>
       <c r="B51" s="75" t="s">
         <v>340</v>
@@ -16605,7 +16605,7 @@
       </c>
       <c r="P51" s="77"/>
     </row>
-    <row r="52" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A52" s="69"/>
       <c r="B52" s="75" t="s">
         <v>345</v>
@@ -16641,7 +16641,7 @@
       <c r="O52" s="77"/>
       <c r="P52" s="77"/>
     </row>
-    <row r="53" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A53" s="69"/>
       <c r="B53" s="75" t="s">
         <v>345</v>
@@ -16677,7 +16677,7 @@
       <c r="O53" s="77"/>
       <c r="P53" s="77"/>
     </row>
-    <row r="54" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A54" s="69"/>
       <c r="B54" s="75" t="s">
         <v>345</v>
@@ -16713,7 +16713,7 @@
       <c r="O54" s="77"/>
       <c r="P54" s="77"/>
     </row>
-    <row r="55" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A55" s="69"/>
       <c r="B55" s="75" t="s">
         <v>351</v>
@@ -16749,7 +16749,7 @@
       <c r="O55" s="77"/>
       <c r="P55" s="77"/>
     </row>
-    <row r="56" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A56" s="69"/>
       <c r="B56" s="75" t="s">
         <v>351</v>
@@ -16785,7 +16785,7 @@
       <c r="O56" s="77"/>
       <c r="P56" s="77"/>
     </row>
-    <row r="57" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A57" s="69"/>
       <c r="B57" s="75" t="s">
         <v>357</v>
@@ -16821,7 +16821,7 @@
       <c r="O57" s="77"/>
       <c r="P57" s="77"/>
     </row>
-    <row r="58" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A58" s="69"/>
       <c r="B58" s="75" t="s">
         <v>357</v>
@@ -16857,7 +16857,7 @@
       <c r="O58" s="77"/>
       <c r="P58" s="77"/>
     </row>
-    <row r="59" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A59" s="69"/>
       <c r="B59" s="75" t="s">
         <v>357</v>
@@ -16893,7 +16893,7 @@
       <c r="O59" s="77"/>
       <c r="P59" s="77"/>
     </row>
-    <row r="60" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A60" s="69"/>
       <c r="B60" s="75" t="s">
         <v>357</v>
@@ -16929,7 +16929,7 @@
       <c r="O60" s="77"/>
       <c r="P60" s="77"/>
     </row>
-    <row r="61" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A61" s="69"/>
       <c r="B61" s="75" t="s">
         <v>372</v>
@@ -16965,7 +16965,7 @@
       <c r="O61" s="77"/>
       <c r="P61" s="77"/>
     </row>
-    <row r="62" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A62" s="69"/>
       <c r="B62" s="75" t="s">
         <v>597</v>
@@ -17001,7 +17001,7 @@
       <c r="O62" s="77"/>
       <c r="P62" s="77"/>
     </row>
-    <row r="63" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A63" s="69"/>
       <c r="B63" s="75" t="s">
         <v>380</v>
@@ -17037,7 +17037,7 @@
       <c r="O63" s="77"/>
       <c r="P63" s="77"/>
     </row>
-    <row r="64" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A64" s="69"/>
       <c r="B64" s="75" t="s">
         <v>390</v>
@@ -17075,7 +17075,7 @@
       </c>
       <c r="P64" s="77"/>
     </row>
-    <row r="65" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A65" s="69"/>
       <c r="B65" s="75" t="s">
         <v>392</v>
@@ -17113,7 +17113,7 @@
       <c r="O65" s="77"/>
       <c r="P65" s="77"/>
     </row>
-    <row r="66" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A66" s="69"/>
       <c r="B66" s="75" t="s">
         <v>392</v>
@@ -17149,7 +17149,7 @@
       <c r="O66" s="77"/>
       <c r="P66" s="77"/>
     </row>
-    <row r="67" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A67" s="69"/>
       <c r="B67" s="75" t="s">
         <v>396</v>
@@ -17185,7 +17185,7 @@
       <c r="O67" s="77"/>
       <c r="P67" s="77"/>
     </row>
-    <row r="68" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A68" s="69"/>
       <c r="B68" s="75" t="s">
         <v>396</v>
@@ -17221,7 +17221,7 @@
       <c r="O68" s="77"/>
       <c r="P68" s="77"/>
     </row>
-    <row r="69" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A69" s="69"/>
       <c r="B69" s="75" t="s">
         <v>396</v>
@@ -17257,7 +17257,7 @@
       <c r="O69" s="77"/>
       <c r="P69" s="77"/>
     </row>
-    <row r="70" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A70" s="69"/>
       <c r="B70" s="75" t="s">
         <v>600</v>
@@ -17293,7 +17293,7 @@
       <c r="O70" s="77"/>
       <c r="P70" s="77"/>
     </row>
-    <row r="71" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A71" s="69"/>
       <c r="B71" s="75" t="s">
         <v>410</v>
@@ -17329,7 +17329,7 @@
       <c r="O71" s="77"/>
       <c r="P71" s="77"/>
     </row>
-    <row r="72" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A72" s="69"/>
       <c r="B72" s="75" t="s">
         <v>412</v>
@@ -17365,7 +17365,7 @@
       <c r="O72" s="77"/>
       <c r="P72" s="77"/>
     </row>
-    <row r="73" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A73" s="69"/>
       <c r="B73" s="75" t="s">
         <v>417</v>
@@ -17401,7 +17401,7 @@
       <c r="O73" s="78"/>
       <c r="P73" s="78"/>
     </row>
-    <row r="74" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A74" s="69"/>
       <c r="B74" s="75" t="s">
         <v>427</v>
@@ -17439,7 +17439,7 @@
       </c>
       <c r="P74" s="77"/>
     </row>
-    <row r="75" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A75" s="69"/>
       <c r="B75" s="75" t="s">
         <v>430</v>
@@ -17475,7 +17475,7 @@
       <c r="O75" s="77"/>
       <c r="P75" s="77"/>
     </row>
-    <row r="76" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A76" s="69"/>
       <c r="B76" s="75" t="s">
         <v>433</v>
@@ -17511,7 +17511,7 @@
       <c r="O76" s="77"/>
       <c r="P76" s="77"/>
     </row>
-    <row r="77" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A77" s="69"/>
       <c r="B77" s="75" t="s">
         <v>433</v>
@@ -17547,7 +17547,7 @@
       <c r="O77" s="77"/>
       <c r="P77" s="77"/>
     </row>
-    <row r="78" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A78" s="69"/>
       <c r="B78" s="75" t="s">
         <v>442</v>
@@ -17583,7 +17583,7 @@
       <c r="O78" s="77"/>
       <c r="P78" s="77"/>
     </row>
-    <row r="79" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A79" s="69"/>
       <c r="B79" s="75" t="s">
         <v>442</v>
@@ -17621,7 +17621,7 @@
       </c>
       <c r="P79" s="77"/>
     </row>
-    <row r="80" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A80" s="69"/>
       <c r="B80" s="75" t="s">
         <v>442</v>
@@ -17657,7 +17657,7 @@
       <c r="O80" s="77"/>
       <c r="P80" s="77"/>
     </row>
-    <row r="81" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A81" s="69"/>
       <c r="B81" s="75" t="s">
         <v>442</v>
@@ -17693,7 +17693,7 @@
       <c r="O81" s="77"/>
       <c r="P81" s="77"/>
     </row>
-    <row r="82" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A82" s="69"/>
       <c r="B82" s="75" t="s">
         <v>442</v>
@@ -17729,7 +17729,7 @@
       <c r="O82" s="77"/>
       <c r="P82" s="77"/>
     </row>
-    <row r="83" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A83" s="69"/>
       <c r="B83" s="75" t="s">
         <v>442</v>
@@ -17765,7 +17765,7 @@
       <c r="O83" s="77"/>
       <c r="P83" s="77"/>
     </row>
-    <row r="84" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A84" s="69"/>
       <c r="B84" s="75" t="s">
         <v>451</v>
@@ -17801,7 +17801,7 @@
       <c r="O84" s="77"/>
       <c r="P84" s="77"/>
     </row>
-    <row r="85" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A85" s="69"/>
       <c r="B85" s="75" t="s">
         <v>456</v>
@@ -17837,7 +17837,7 @@
       <c r="O85" s="77"/>
       <c r="P85" s="77"/>
     </row>
-    <row r="86" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A86" s="69"/>
       <c r="B86" s="75" t="s">
         <v>459</v>
@@ -17884,7 +17884,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="87" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A87" s="69"/>
       <c r="B87" s="75" t="s">
         <v>421</v>
@@ -17920,7 +17920,7 @@
       <c r="O87" s="77"/>
       <c r="P87" s="77"/>
     </row>
-    <row r="88" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A88" s="69"/>
       <c r="B88" s="75" t="s">
         <v>421</v>
@@ -17956,7 +17956,7 @@
       <c r="O88" s="77"/>
       <c r="P88" s="77"/>
     </row>
-    <row r="89" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A89" s="69"/>
       <c r="B89" s="75" t="s">
         <v>608</v>
@@ -17992,7 +17992,7 @@
       <c r="O89" s="77"/>
       <c r="P89" s="77"/>
     </row>
-    <row r="90" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A90" s="69"/>
       <c r="B90" s="75" t="s">
         <v>466</v>
@@ -18028,7 +18028,7 @@
       <c r="O90" s="77"/>
       <c r="P90" s="77"/>
     </row>
-    <row r="91" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A91" s="69"/>
       <c r="B91" s="75" t="s">
         <v>466</v>
@@ -18064,7 +18064,7 @@
       <c r="O91" s="77"/>
       <c r="P91" s="77"/>
     </row>
-    <row r="92" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A92" s="69"/>
       <c r="B92" s="75" t="s">
         <v>466</v>
@@ -18100,7 +18100,7 @@
       <c r="O92" s="77"/>
       <c r="P92" s="77"/>
     </row>
-    <row r="93" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A93" s="69"/>
       <c r="B93" s="75" t="s">
         <v>466</v>
@@ -18149,7 +18149,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="94" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A94" s="69"/>
       <c r="B94" s="75" t="s">
         <v>610</v>
@@ -18185,7 +18185,7 @@
       <c r="O94" s="77"/>
       <c r="P94" s="77"/>
     </row>
-    <row r="95" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A95" s="69"/>
       <c r="B95" s="75" t="s">
         <v>612</v>
@@ -18221,7 +18221,7 @@
       <c r="O95" s="77"/>
       <c r="P95" s="77"/>
     </row>
-    <row r="96" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A96" s="69"/>
       <c r="B96" s="75" t="s">
         <v>614</v>
@@ -18257,7 +18257,7 @@
       <c r="O96" s="77"/>
       <c r="P96" s="77"/>
     </row>
-    <row r="97" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A97" s="69"/>
       <c r="B97" s="75" t="s">
         <v>614</v>
@@ -18298,7 +18298,7 @@
       <c r="O97" s="77"/>
       <c r="P97" s="77"/>
     </row>
-    <row r="98" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A98" s="69"/>
       <c r="B98" s="75" t="s">
         <v>616</v>
@@ -18334,7 +18334,7 @@
       <c r="O98" s="77"/>
       <c r="P98" s="77"/>
     </row>
-    <row r="99" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A99" s="69"/>
       <c r="B99" s="75" t="s">
         <v>473</v>
@@ -18370,7 +18370,7 @@
       <c r="O99" s="77"/>
       <c r="P99" s="77"/>
     </row>
-    <row r="100" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A100" s="69"/>
       <c r="B100" s="75" t="s">
         <v>618</v>
@@ -18406,7 +18406,7 @@
       <c r="O100" s="77"/>
       <c r="P100" s="77"/>
     </row>
-    <row r="101" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A101" s="69"/>
       <c r="B101" s="75" t="s">
         <v>619</v>
@@ -18442,7 +18442,7 @@
       <c r="O101" s="77"/>
       <c r="P101" s="77"/>
     </row>
-    <row r="102" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A102" s="69"/>
       <c r="B102" s="75" t="s">
         <v>619</v>
@@ -18478,7 +18478,7 @@
       <c r="O102" s="77"/>
       <c r="P102" s="77"/>
     </row>
-    <row r="103" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A103" s="69"/>
       <c r="B103" s="75" t="s">
         <v>476</v>
@@ -18514,7 +18514,7 @@
       <c r="O103" s="77"/>
       <c r="P103" s="77"/>
     </row>
-    <row r="104" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A104" s="69"/>
       <c r="B104" s="75" t="s">
         <v>476</v>
@@ -18550,7 +18550,7 @@
       <c r="O104" s="77"/>
       <c r="P104" s="77"/>
     </row>
-    <row r="105" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A105" s="69"/>
       <c r="B105" s="75" t="s">
         <v>482</v>
@@ -18586,7 +18586,7 @@
       <c r="O105" s="77"/>
       <c r="P105" s="77"/>
     </row>
-    <row r="106" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A106" s="69"/>
       <c r="B106" s="75" t="s">
         <v>635</v>
@@ -18622,7 +18622,7 @@
       <c r="O106" s="77"/>
       <c r="P106" s="77"/>
     </row>
-    <row r="107" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A107" s="69"/>
       <c r="B107" s="75" t="s">
         <v>636</v>
@@ -18658,7 +18658,7 @@
       <c r="O107" s="77"/>
       <c r="P107" s="77"/>
     </row>
-    <row r="108" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A108" s="69"/>
       <c r="B108" s="75" t="s">
         <v>638</v>
@@ -18694,7 +18694,7 @@
       <c r="O108" s="77"/>
       <c r="P108" s="77"/>
     </row>
-    <row r="109" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A109" s="69"/>
       <c r="B109" s="75" t="s">
         <v>640</v>
@@ -18730,7 +18730,7 @@
       <c r="O109" s="77"/>
       <c r="P109" s="77"/>
     </row>
-    <row r="110" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A110" s="69"/>
       <c r="B110" s="75" t="s">
         <v>643</v>
@@ -18766,7 +18766,7 @@
       <c r="O110" s="77"/>
       <c r="P110" s="77"/>
     </row>
-    <row r="111" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A111" s="69"/>
       <c r="B111" s="75" t="s">
         <v>644</v>
@@ -18802,7 +18802,7 @@
       <c r="O111" s="77"/>
       <c r="P111" s="77"/>
     </row>
-    <row r="112" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A112" s="69"/>
       <c r="B112" s="75" t="s">
         <v>488</v>
@@ -18838,7 +18838,7 @@
       <c r="O112" s="77"/>
       <c r="P112" s="77"/>
     </row>
-    <row r="113" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A113" s="69"/>
       <c r="B113" s="75" t="s">
         <v>491</v>
@@ -18874,7 +18874,7 @@
       <c r="O113" s="77"/>
       <c r="P113" s="77"/>
     </row>
-    <row r="114" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A114" s="69"/>
       <c r="B114" s="75" t="s">
         <v>379</v>
@@ -18910,7 +18910,7 @@
       <c r="O114" s="77"/>
       <c r="P114" s="77"/>
     </row>
-    <row r="115" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A115" s="69"/>
       <c r="B115" s="75" t="s">
         <v>499</v>
@@ -18946,7 +18946,7 @@
       <c r="O115" s="77"/>
       <c r="P115" s="77"/>
     </row>
-    <row r="116" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A116" s="69"/>
       <c r="B116" s="75" t="s">
         <v>499</v>
@@ -18982,7 +18982,7 @@
       <c r="O116" s="77"/>
       <c r="P116" s="77"/>
     </row>
-    <row r="117" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A117" s="69"/>
       <c r="B117" s="75" t="s">
         <v>503</v>
@@ -19018,7 +19018,7 @@
       <c r="O117" s="77"/>
       <c r="P117" s="77"/>
     </row>
-    <row r="118" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A118" s="69"/>
       <c r="B118" s="75" t="s">
         <v>669</v>
@@ -19054,7 +19054,7 @@
       <c r="O118" s="77"/>
       <c r="P118" s="77"/>
     </row>
-    <row r="119" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A119" s="69"/>
       <c r="B119" s="75" t="s">
         <v>669</v>
@@ -19090,7 +19090,7 @@
       <c r="O119" s="77"/>
       <c r="P119" s="77"/>
     </row>
-    <row r="120" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A120" s="69"/>
       <c r="B120" s="75" t="s">
         <v>669</v>
@@ -19128,7 +19128,7 @@
       <c r="O120" s="77"/>
       <c r="P120" s="77"/>
     </row>
-    <row r="121" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A121" s="69"/>
       <c r="B121" s="75" t="s">
         <v>669</v>
@@ -19164,7 +19164,7 @@
       <c r="O121" s="77"/>
       <c r="P121" s="77"/>
     </row>
-    <row r="122" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A122" s="69"/>
       <c r="B122" s="75" t="s">
         <v>507</v>
@@ -19200,7 +19200,7 @@
       <c r="O122" s="77"/>
       <c r="P122" s="77"/>
     </row>
-    <row r="123" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A123" s="69"/>
       <c r="B123" s="75" t="s">
         <v>510</v>
@@ -19236,7 +19236,7 @@
       <c r="O123" s="77"/>
       <c r="P123" s="77"/>
     </row>
-    <row r="124" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A124" s="69"/>
       <c r="B124" s="75" t="s">
         <v>512</v>
@@ -19272,7 +19272,7 @@
       <c r="O124" s="77"/>
       <c r="P124" s="77"/>
     </row>
-    <row r="125" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A125" s="69"/>
       <c r="B125" s="75" t="s">
         <v>514</v>
@@ -19308,7 +19308,7 @@
       <c r="O125" s="77"/>
       <c r="P125" s="77"/>
     </row>
-    <row r="126" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A126" s="69"/>
       <c r="B126" s="75" t="s">
         <v>514</v>
@@ -19344,7 +19344,7 @@
       <c r="O126" s="77"/>
       <c r="P126" s="77"/>
     </row>
-    <row r="127" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A127" s="69"/>
       <c r="B127" s="75" t="s">
         <v>519</v>
@@ -19380,7 +19380,7 @@
       <c r="O127" s="77"/>
       <c r="P127" s="77"/>
     </row>
-    <row r="128" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A128" s="69"/>
       <c r="B128" s="75" t="s">
         <v>519</v>
@@ -19421,7 +19421,7 @@
       <c r="O128" s="77"/>
       <c r="P128" s="77"/>
     </row>
-    <row r="129" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A129" s="69"/>
       <c r="B129" s="75" t="s">
         <v>523</v>
@@ -19457,7 +19457,7 @@
       <c r="O129" s="77"/>
       <c r="P129" s="77"/>
     </row>
-    <row r="130" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A130" s="69"/>
       <c r="B130" s="75" t="s">
         <v>523</v>
@@ -19493,7 +19493,7 @@
       <c r="O130" s="77"/>
       <c r="P130" s="77"/>
     </row>
-    <row r="131" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A131" s="69"/>
       <c r="B131" s="75" t="s">
         <v>529</v>
@@ -19529,7 +19529,7 @@
       <c r="O131" s="77"/>
       <c r="P131" s="77"/>
     </row>
-    <row r="132" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A132" s="69"/>
       <c r="B132" s="75" t="s">
         <v>532</v>
@@ -19565,7 +19565,7 @@
       <c r="O132" s="77"/>
       <c r="P132" s="77"/>
     </row>
-    <row r="133" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A133" s="69"/>
       <c r="B133" s="75" t="s">
         <v>649</v>
@@ -19601,7 +19601,7 @@
       <c r="O133" s="77"/>
       <c r="P133" s="77"/>
     </row>
-    <row r="134" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A134" s="69"/>
       <c r="B134" s="75" t="s">
         <v>534</v>
@@ -19637,7 +19637,7 @@
       <c r="O134" s="77"/>
       <c r="P134" s="77"/>
     </row>
-    <row r="135" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A135" s="69"/>
       <c r="B135" s="75" t="s">
         <v>534</v>
@@ -19673,7 +19673,7 @@
       <c r="O135" s="77"/>
       <c r="P135" s="77"/>
     </row>
-    <row r="136" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A136" s="69"/>
       <c r="B136" s="75" t="s">
         <v>552</v>
@@ -19709,7 +19709,7 @@
       <c r="O136" s="77"/>
       <c r="P136" s="77"/>
     </row>
-    <row r="137" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A137" s="69"/>
       <c r="B137" s="75" t="s">
         <v>554</v>
@@ -19745,7 +19745,7 @@
       <c r="O137" s="77"/>
       <c r="P137" s="77"/>
     </row>
-    <row r="138" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A138" s="69"/>
       <c r="B138" s="75" t="s">
         <v>556</v>
@@ -19781,7 +19781,7 @@
       <c r="O138" s="77"/>
       <c r="P138" s="77"/>
     </row>
-    <row r="139" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A139" s="69"/>
       <c r="B139" s="75" t="s">
         <v>561</v>
@@ -19817,7 +19817,7 @@
       <c r="O139" s="77"/>
       <c r="P139" s="77"/>
     </row>
-    <row r="140" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A140" s="69"/>
       <c r="B140" s="75" t="s">
         <v>561</v>
@@ -19853,7 +19853,7 @@
       <c r="O140" s="77"/>
       <c r="P140" s="77"/>
     </row>
-    <row r="141" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A141" s="69"/>
       <c r="B141" s="75" t="s">
         <v>570</v>
@@ -19889,7 +19889,7 @@
       <c r="O141" s="77"/>
       <c r="P141" s="77"/>
     </row>
-    <row r="142" spans="1:16" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A142" s="69"/>
       <c r="B142" s="75" t="s">
         <v>576</v>
@@ -19925,7 +19925,7 @@
       <c r="O142" s="77"/>
       <c r="P142" s="77"/>
     </row>
-    <row r="143" spans="1:16" ht="12" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A143" s="69"/>
       <c r="B143" s="75" t="s">
         <v>578</v>
@@ -19961,7 +19961,7 @@
       <c r="O143" s="77"/>
       <c r="P143" s="77"/>
     </row>
-    <row r="144" spans="1:16" ht="21.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:16" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A144" s="69"/>
       <c r="B144" s="75" t="s">
         <v>578</v>
@@ -19997,7 +19997,7 @@
       <c r="O144" s="77"/>
       <c r="P144" s="77"/>
     </row>
-    <row r="145" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A145" s="80">
         <v>124075</v>
       </c>
@@ -20049,7 +20049,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="146" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A146" s="80">
         <v>126284</v>
       </c>
@@ -20100,7 +20100,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="147" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A147" s="80">
         <v>127053</v>
       </c>
@@ -20127,7 +20127,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="148" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A148" s="69">
         <v>102150</v>
       </c>
@@ -20173,7 +20173,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="149" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A149" s="80">
         <v>127112</v>
       </c>
@@ -20225,7 +20225,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="150" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A150" s="69">
         <v>102310</v>
       </c>
@@ -20271,7 +20271,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="151" spans="1:17" s="5" customFormat="1" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:17" s="5" customFormat="1" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A151" s="69">
         <v>102500</v>
       </c>
@@ -20322,7 +20322,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="152" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A152" s="80">
         <v>127899</v>
       </c>
@@ -20374,7 +20374,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="153" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A153" s="80">
         <v>128844</v>
       </c>
@@ -20426,7 +20426,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="154" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A154" s="80">
         <v>131728</v>
       </c>
@@ -20477,7 +20477,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="155" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A155" s="80">
         <v>131736</v>
       </c>
@@ -20529,7 +20529,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="156" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:17" ht="14.5" x14ac:dyDescent="0.25">
       <c r="A156" s="80">
         <v>132042</v>
       </c>
@@ -20556,7 +20556,7 @@
         <v>201812</v>
       </c>
     </row>
-    <row r="157" spans="1:17" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:17" ht="27.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A157" s="80">
         <v>132360</v>
       </c>
@@ -26114,7 +26114,7 @@
   </sheetData>
   <autoFilter ref="A1:P275">
     <filterColumn colId="8">
-      <filters blank="1">
+      <filters>
         <filter val="31/12/208"/>
       </filters>
     </filterColumn>
@@ -29676,18 +29676,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -29823,6 +29823,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1FDE5BE-AC7C-4D1B-A50A-0AAF91DD9714}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52ED17B2-B282-46DB-AB0C-1D336182C094}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
@@ -29834,14 +29842,6 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A1FDE5BE-AC7C-4D1B-A50A-0AAF91DD9714}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>